<commit_message>
mongo vscode extension setup
</commit_message>
<xml_diff>
--- a/June2023/JuneIssues.xlsx
+++ b/June2023/JuneIssues.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>No of days calculation from date of Birth</t>
   </si>
@@ -80,9 +80,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>row bootstrap class css</t>
-  </si>
-  <si>
     <t>Aggregation Vs Composition Vs Association</t>
   </si>
   <si>
@@ -111,6 +108,15 @@
   </si>
   <si>
     <t>Categories CRUD</t>
+  </si>
+  <si>
+    <t>Row bootstrap class css</t>
+  </si>
+  <si>
+    <t>We need to speicify order of the element to  take it to first like order-first class in bootstrap</t>
+  </si>
+  <si>
+    <t>Countries, Cities, CityAreas Tables</t>
   </si>
 </sst>
 </file>
@@ -160,9 +166,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,19 +452,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1"/>
+    </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
@@ -471,6 +483,12 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -481,7 +499,7 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -542,57 +560,62 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>